<commit_message>
Corrige fallos en generación de incidencias
</commit_message>
<xml_diff>
--- a/guia/requisitos.xlsx
+++ b/guia/requisitos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -271,18 +271,18 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="53.4591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="52.780612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>